<commit_message>
Updated planning for Koen&Djordy
</commit_message>
<xml_diff>
--- a/planning/Planning sprint 1.xlsx
+++ b/planning/Planning sprint 1.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21206"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5C867F6-EDAD-4F3E-A0B9-4D436C0A5C21}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djord\Desktop\hz\1rd-GameDev\planning\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB4F6E8-DEF8-4462-80EF-6BC3FAAFC91E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -106,7 +104,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,7 +314,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -614,21 +612,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="7" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="7" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -657,7 +655,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>43444</v>
       </c>
@@ -682,7 +680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>43444</v>
       </c>
@@ -696,7 +694,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -707,7 +705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>43444</v>
       </c>
@@ -721,7 +719,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -732,7 +730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>43444</v>
       </c>
@@ -757,7 +755,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>43444</v>
       </c>
@@ -771,7 +769,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -782,7 +780,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>43445</v>
       </c>
@@ -807,7 +805,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>43445</v>
       </c>
@@ -832,7 +830,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>43445</v>
       </c>
@@ -854,7 +852,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <v>43446</v>
       </c>
@@ -874,7 +872,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -886,7 +884,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -898,7 +896,7 @@
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -910,7 +908,7 @@
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="11"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -922,7 +920,7 @@
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -934,7 +932,7 @@
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -946,7 +944,7 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -958,7 +956,7 @@
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -970,7 +968,7 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -982,7 +980,7 @@
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -994,7 +992,7 @@
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
     </row>
   </sheetData>

</xml_diff>